<commit_message>
add main BoM and images
</commit_message>
<xml_diff>
--- a/documentation/bom/Basic-DC-mixer-bom.xlsx
+++ b/documentation/bom/Basic-DC-mixer-bom.xlsx
@@ -194,13 +194,13 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-01-14_11-35-36</t>
+    <t>2023-06-10_15-38-43</t>
   </si>
   <si>
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.10+dfsg-1~bpo11+1</t>
+    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -392,7 +392,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -407,7 +407,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -730,7 +739,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="54.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
@@ -907,7 +916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30.0" customHeight="1">
+    <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30.0" customHeight="1">
+    <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>